<commit_message>
* updated with template that was forgotten
</commit_message>
<xml_diff>
--- a/Items/Templates/Email usage and descriptions.xlsx
+++ b/Items/Templates/Email usage and descriptions.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="170">
   <si>
     <t>Internal</t>
   </si>
@@ -520,6 +520,12 @@
   </si>
   <si>
     <t xml:space="preserve">Underwriter sidebar -&gt; email "Resend confirmation" or change email button </t>
+  </si>
+  <si>
+    <t>Debit card billed but no money in the account</t>
+  </si>
+  <si>
+    <t>Debit card repayment failure</t>
   </si>
 </sst>
 </file>
@@ -1008,10 +1014,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J49"/>
+  <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1839,6 +1845,23 @@
       </c>
       <c r="E49" s="2" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A50" s="2">
+        <v>46</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- EZ-388 obsolete items
</commit_message>
<xml_diff>
--- a/Items/Templates/Email usage and descriptions.xlsx
+++ b/Items/Templates/Email usage and descriptions.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="164">
   <si>
     <t>Internal</t>
   </si>
@@ -36,9 +36,6 @@
     <t>Comment</t>
   </si>
   <si>
-    <t>DS Exception.docx</t>
-  </si>
-  <si>
     <t>DS Exception without umi</t>
   </si>
   <si>
@@ -66,9 +63,6 @@
     <t>Data Source crashed</t>
   </si>
   <si>
-    <t>Obsolete</t>
-  </si>
-  <si>
     <t>Strategy</t>
   </si>
   <si>
@@ -99,15 +93,6 @@
     <t>Shops are not Updated yet</t>
   </si>
   <si>
-    <t>Pay early and save</t>
-  </si>
-  <si>
-    <t>TwoWeeksDueMail</t>
-  </si>
-  <si>
-    <t>Early Payment Offer</t>
-  </si>
-  <si>
     <t>Underwriter added a debit card</t>
   </si>
   <si>
@@ -514,9 +499,6 @@
   </si>
   <si>
     <t>When trying to charge money at 8 AM, the script node that charges money from customers has crashed</t>
-  </si>
-  <si>
-    <t>sends an email for Two Weeks due loansd. Has 80% of logic implemented, but not used in the system, instead of this one we use FiveDaysDue logic</t>
   </si>
   <si>
     <t xml:space="preserve">Underwriter sidebar -&gt; email "Resend confirmation" or change email button </t>
@@ -1017,7 +999,7 @@
   <dimension ref="A1:J50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E51" sqref="E51"/>
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1033,7 +1015,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>2</v>
@@ -1045,7 +1027,7 @@
         <v>4</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>5</v>
@@ -1068,16 +1050,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1085,16 +1067,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1102,16 +1084,16 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -1119,16 +1101,16 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -1136,16 +1118,16 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -1153,16 +1135,16 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -1170,16 +1152,16 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -1187,16 +1169,16 @@
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -1204,16 +1186,16 @@
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1221,19 +1203,19 @@
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -1241,16 +1223,16 @@
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -1258,16 +1240,16 @@
         <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1275,16 +1257,16 @@
         <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1292,16 +1274,16 @@
         <v>14</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1309,16 +1291,16 @@
         <v>15</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1326,16 +1308,16 @@
         <v>16</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1343,16 +1325,16 @@
         <v>17</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1360,16 +1342,16 @@
         <v>18</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1377,16 +1359,16 @@
         <v>19</v>
       </c>
       <c r="B21" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>123</v>
-      </c>
       <c r="E21" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1394,16 +1376,16 @@
         <v>20</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1411,16 +1393,16 @@
         <v>21</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1428,16 +1410,16 @@
         <v>22</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1445,16 +1427,16 @@
         <v>23</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1462,16 +1444,16 @@
         <v>24</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1479,16 +1461,16 @@
         <v>25</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1496,16 +1478,16 @@
         <v>26</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1513,16 +1495,16 @@
         <v>27</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1530,16 +1512,16 @@
         <v>28</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1547,16 +1529,16 @@
         <v>29</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1567,301 +1549,267 @@
       <c r="D32" s="6"/>
       <c r="E32" s="6"/>
     </row>
-    <row r="33" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>30</v>
       </c>
       <c r="B33" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="D33" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D33" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="E33" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>31</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C34" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D34" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D34" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="E34" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>32</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C35" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D35" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D35" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="E35" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>33</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>34</v>
       </c>
       <c r="B37" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D37" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C37" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>39</v>
-      </c>
       <c r="E37" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>35</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>36</v>
       </c>
       <c r="B39" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C39" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="D39" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>37</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>38</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>39</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>40</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>41</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>42</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B46" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C46" s="8"/>
       <c r="D46" s="8"/>
       <c r="E46" s="9"/>
     </row>
-    <row r="47" spans="1:6" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>43</v>
       </c>
       <c r="B47" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C47" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C47" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="D47" s="2" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="2">
-        <v>44</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E48" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F48" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A49" s="2">
-        <v>45</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>28</v>
-      </c>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E48" s="3"/>
     </row>
     <row r="50" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>46</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>